<commit_message>
Javitottam az excel fajlt
</commit_message>
<xml_diff>
--- a/Alkatreszek.xlsx
+++ b/Alkatreszek.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\László\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\László\Desktop\PCsim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F496BB6F-48AE-4F33-AD2E-DC1C32E06D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86964E8D-EC9E-49ED-A259-37813A4632C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{31FDE73E-6992-4C86-B7FA-3436D67663FF}"/>
   </bookViews>
@@ -426,7 +426,7 @@
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;Ft&quot;;[Red]\-#,##0\ &quot;Ft&quot;"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;Ft&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -451,6 +451,14 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -644,63 +652,33 @@
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -710,8 +688,38 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1029,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A344E04B-8186-4850-8E3B-A1C9DE899D1E}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A58" sqref="A2:A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,681 +1054,673 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="13"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="22">
         <v>32690</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="6" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="6" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="6" t="s">
+      <c r="A9" s="26"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="9" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="22">
         <v>28790</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="6" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="6" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="6" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="6" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="6" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="6" t="s">
+      <c r="A17" s="26"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="6" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="6" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="6" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="6" t="s">
+      <c r="A21" s="26"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="6" t="s">
+      <c r="A22" s="26"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="6" t="s">
+      <c r="A23" s="26"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="6" t="s">
+      <c r="A24" s="26"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="6" t="s">
+      <c r="A25" s="26"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="6" t="s">
+      <c r="A26" s="26"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="9" t="s">
+      <c r="A27" s="27"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="7" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="14">
         <v>24290</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="6" t="s">
+      <c r="A29" s="26"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="6" t="s">
+      <c r="A30" s="26"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="6" t="s">
+      <c r="A31" s="26"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="6" t="s">
+      <c r="A32" s="26"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="6" t="s">
+      <c r="A33" s="26"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="6" t="s">
+      <c r="A34" s="26"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="5" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="6" t="s">
+      <c r="A35" s="26"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="9" t="s">
+      <c r="A36" s="27"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="10"/>
+      <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="18">
+      <c r="B37" s="14">
         <v>83790</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="25" t="s">
+      <c r="A38" s="29"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="5" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="25" t="s">
+      <c r="A39" s="29"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="25" t="s">
+      <c r="A40" s="29"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="5" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="25" t="s">
+      <c r="A41" s="29"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="25" t="s">
+      <c r="A42" s="29"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="26" t="s">
+      <c r="A43" s="30"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="7" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="18">
+      <c r="B44" s="14">
         <v>14190</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="C44" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="3" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="25" t="s">
+      <c r="A45" s="29"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="25" t="s">
+      <c r="A46" s="29"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="26" t="s">
+      <c r="A47" s="30"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D47" s="10"/>
+      <c r="D47" s="7"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="18">
+      <c r="B48" s="14">
         <v>188490</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="25" t="s">
+      <c r="A49" s="29"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="25" t="s">
+      <c r="A50" s="29"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="5" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="25" t="s">
+      <c r="A51" s="29"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="5" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="25" t="s">
+      <c r="A52" s="29"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="25" t="s">
+      <c r="A53" s="29"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="5" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="23"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="26" t="s">
+      <c r="A54" s="30"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="7" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B55" s="18">
+      <c r="B55" s="14">
         <v>16990</v>
       </c>
-      <c r="C55" s="24" t="s">
+      <c r="C55" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="22"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="25" t="s">
+      <c r="A56" s="29"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="23"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="25" t="s">
+      <c r="A57" s="30"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="21" t="s">
+      <c r="A58" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B58" s="27">
+      <c r="B58" s="17">
         <v>13090</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="C58" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
-      <c r="B59" s="28"/>
-      <c r="C59" s="25" t="s">
+      <c r="A59" s="29"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="28"/>
-      <c r="C60" s="25" t="s">
+      <c r="A60" s="29"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="25" t="s">
+      <c r="A61" s="29"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
-      <c r="B62" s="28"/>
-      <c r="C62" s="25" t="s">
+      <c r="A62" s="29"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="23"/>
-      <c r="B63" s="29"/>
-      <c r="C63" s="26" t="s">
+      <c r="A63" s="30"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D63" s="10"/>
+      <c r="D63" s="7"/>
     </row>
     <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="30">
+      <c r="B64" s="13">
         <f>SUM(B2:B58)</f>
         <v>402320</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A28:A36"/>
-    <mergeCell ref="B28:B36"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B47"/>
     <mergeCell ref="A58:A63"/>
     <mergeCell ref="B58:B63"/>
     <mergeCell ref="C1:D1"/>
@@ -1730,6 +1730,14 @@
     <mergeCell ref="A11:A27"/>
     <mergeCell ref="A55:A57"/>
     <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B48:B54"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="A28:A36"/>
+    <mergeCell ref="B28:B36"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B47"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>